<commit_message>
Update Excel files b2m.xlsx and b3f.xlsx with new tournament data. These changes include updated match schedules and game statuses to reflect the latest tournament management requirements.
</commit_message>
<xml_diff>
--- a/b2m.xlsx
+++ b/b2m.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SynologyDrive\Python\Varia\beach_tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994496D5-1B60-48AC-86F1-F6CB225EFCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578379F3-8955-49C1-89C1-3F83101D9EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55690" yWindow="1630" windowWidth="37230" windowHeight="18430" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48920" yWindow="2360" windowWidth="37230" windowHeight="18430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Anmeldung" sheetId="4" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="102">
   <si>
     <t>Seed</t>
   </si>
@@ -308,12 +308,6 @@
     <t>Luc</t>
   </si>
   <si>
-    <t>Dürst</t>
-  </si>
-  <si>
-    <t>Linus</t>
-  </si>
-  <si>
     <t>Hill Azpeitia</t>
   </si>
   <si>
@@ -386,9 +380,6 @@
     <t>Yanis</t>
   </si>
   <si>
-    <t>Marwin</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -396,6 +387,9 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>bye</t>
   </si>
 </sst>
 </file>
@@ -404,7 +398,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="h:mm"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1346,7 +1340,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1748,8 +1742,8 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1821,10 +1815,10 @@
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1855,10 +1849,10 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1889,10 +1883,10 @@
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1923,10 +1917,10 @@
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -1991,10 +1985,10 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2025,10 +2019,10 @@
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -2059,10 +2053,10 @@
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -2127,10 +2121,10 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2161,10 +2155,10 @@
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="38" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2195,10 +2189,10 @@
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2229,7 +2223,7 @@
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14" s="41" t="s">
         <v>41</v>
@@ -2263,10 +2257,10 @@
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2297,10 +2291,10 @@
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -2324,33 +2318,33 @@
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="38" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="58" t="str">
         <f>CONCATENATE($B$17," / ",$E$17)</f>
-        <v>Dürst / Dürst</v>
+        <v>bye / bye</v>
       </c>
       <c r="J17" s="41"/>
       <c r="K17" s="39"/>
       <c r="L17" s="58" t="str">
         <f>CONCATENATE($B$17," / ",$E$17)</f>
-        <v>Dürst / Dürst</v>
+        <v>bye / bye</v>
       </c>
       <c r="M17" s="55" t="str">
         <f>CONCATENATE($C$17," ",$B$17," / ",$F$17," ",$E$17)</f>
-        <v>Linus Dürst / Marwin Dürst</v>
+        <v>bye bye / bye bye</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -2398,7 +2392,7 @@
   <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="15.5" x14ac:dyDescent="0.25"/>
@@ -2488,21 +2482,19 @@
       </c>
       <c r="G2" s="5" t="str">
         <f>IF(Anmeldung!$I$17=" / ",CONCATENATE("Seed #",Anmeldung!$A$17),Anmeldung!$I$17)</f>
-        <v>Dürst / Dürst</v>
-      </c>
-      <c r="H2" s="67" t="str">
-        <f t="shared" ref="H2:H15" si="0">IF(L2=N2,"",SUM(IF(L2&gt;N2,1,0),IF(O2&gt;Q2,1,0),IF(R2&lt;=T2,0,1)))</f>
-        <v/>
+        <v>bye / bye</v>
+      </c>
+      <c r="H2" s="67">
+        <v>2</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="67" t="str">
-        <f t="shared" ref="J2:J15" si="1">IF(L2=N2,"",SUM(IF(L2&lt;N2,1,0),IF(O2&lt;Q2,1,0),IF(R2&gt;=T2,0,1)))</f>
-        <v/>
+      <c r="J2" s="67">
+        <v>0</v>
       </c>
       <c r="K2" s="93">
-        <f t="shared" ref="K2:K15" si="2">SUM(V2-U2)</f>
+        <f t="shared" ref="K2:K15" si="0">SUM(V2-U2)</f>
         <v>0</v>
       </c>
       <c r="L2" s="86"/>
@@ -2527,7 +2519,7 @@
     </row>
     <row r="3" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92">
-        <f t="shared" ref="A3:A31" si="3">SUM(A2,1)</f>
+        <f t="shared" ref="A3:A31" si="1">SUM(A2,1)</f>
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -2551,18 +2543,18 @@
         <v>Charkin / Hrytsuk</v>
       </c>
       <c r="H3" s="67" t="str">
+        <f t="shared" ref="H2:H15" si="2">IF(L3=N3,"",SUM(IF(L3&gt;N3,1,0),IF(O3&gt;Q3,1,0),IF(R3&lt;=T3,0,1)))</f>
+        <v/>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="67" t="str">
+        <f t="shared" ref="J2:J15" si="3">IF(L3=N3,"",SUM(IF(L3&lt;N3,1,0),IF(O3&lt;Q3,1,0),IF(R3&gt;=T3,0,1)))</f>
+        <v/>
+      </c>
+      <c r="K3" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K3" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L3" s="86"/>
@@ -2587,7 +2579,7 @@
     </row>
     <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -2611,18 +2603,18 @@
         <v>Bothen / Arndt</v>
       </c>
       <c r="H4" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K4" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K4" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L4" s="86"/>
@@ -2647,7 +2639,7 @@
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -2669,18 +2661,18 @@
         <v>Pérez / Lendzian</v>
       </c>
       <c r="H5" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K5" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K5" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L5" s="86"/>
@@ -2705,7 +2697,7 @@
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -2727,18 +2719,18 @@
         <v>Ducret / Abassi</v>
       </c>
       <c r="H6" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K6" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K6" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L6" s="86"/>
@@ -2763,7 +2755,7 @@
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -2785,18 +2777,18 @@
         <v>Bosshard / Strebel</v>
       </c>
       <c r="H7" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K7" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K7" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L7" s="86"/>
@@ -2821,7 +2813,7 @@
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -2843,18 +2835,18 @@
         <v>Mikami / Hofmann</v>
       </c>
       <c r="H8" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K8" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K8" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L8" s="86"/>
@@ -2879,7 +2871,7 @@
     </row>
     <row r="9" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -2901,18 +2893,18 @@
         <v>Adamson / Müller</v>
       </c>
       <c r="H9" s="68" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="68" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K9" s="97">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="68" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K9" s="97">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L9" s="104"/>
@@ -2937,7 +2929,7 @@
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="7">
@@ -2947,7 +2939,7 @@
       <c r="D10" s="100"/>
       <c r="E10" s="7" t="str">
         <f>IF($H$2=$J$2,CONCATENATE("Loser Match #",$A$2),IF($H$2&lt;$J$2,$E$2,$G$2))</f>
-        <v>Loser Match #1</v>
+        <v>bye / bye</v>
       </c>
       <c r="F10" s="7" t="s">
         <v>7</v>
@@ -2956,19 +2948,17 @@
         <f>IF($H$3=$J$3,CONCATENATE("Loser Match #",$A$3),IF($H$3&lt;$J$3,$E$3,$G$3))</f>
         <v>Loser Match #2</v>
       </c>
-      <c r="H10" s="69" t="str">
+      <c r="H10" s="69">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="67">
+        <v>2</v>
+      </c>
+      <c r="K10" s="101">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="69" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K10" s="101">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L10" s="102"/>
@@ -2993,7 +2983,7 @@
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B11" s="5">
@@ -3013,18 +3003,18 @@
         <v>Loser Match #4</v>
       </c>
       <c r="H11" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K11" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K11" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L11" s="86"/>
@@ -3049,7 +3039,7 @@
     </row>
     <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B12" s="5">
@@ -3069,18 +3059,18 @@
         <v>Loser Match #6</v>
       </c>
       <c r="H12" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K12" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J12" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K12" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L12" s="86"/>
@@ -3105,7 +3095,7 @@
     </row>
     <row r="13" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="6">
@@ -3125,18 +3115,18 @@
         <v>Loser Match #8</v>
       </c>
       <c r="H13" s="68" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="68" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K13" s="97">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="68" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K13" s="97">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L13" s="104"/>
@@ -3161,7 +3151,7 @@
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3171,7 +3161,7 @@
       <c r="D14" s="100"/>
       <c r="E14" s="7" t="str">
         <f>IF($H$2=$J$2,CONCATENATE("Winner Match #",$A$2),IF($H$2&gt;$J$2,$E$2,$G$2))</f>
-        <v>Winner Match #1</v>
+        <v>Baltermi / Hill Azpeitia</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>7</v>
@@ -3181,18 +3171,18 @@
         <v>Winner Match #2</v>
       </c>
       <c r="H14" s="69" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="69" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K14" s="101">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J14" s="69" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K14" s="101">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L14" s="102"/>
@@ -3217,7 +3207,7 @@
     </row>
     <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -3237,18 +3227,18 @@
         <v>Winner Match #4</v>
       </c>
       <c r="H15" s="67" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="67" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="K15" s="93">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K15" s="93">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L15" s="86"/>
@@ -3273,7 +3263,7 @@
     </row>
     <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -3329,7 +3319,7 @@
     </row>
     <row r="17" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -3385,7 +3375,7 @@
     </row>
     <row r="18" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="7">
@@ -3441,7 +3431,7 @@
     </row>
     <row r="19" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="5">
@@ -3497,7 +3487,7 @@
     </row>
     <row r="20" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="5">
@@ -3553,7 +3543,7 @@
     </row>
     <row r="21" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="6">
@@ -3563,7 +3553,7 @@
       <c r="D21" s="96"/>
       <c r="E21" s="6" t="str">
         <f>IF($H$10=$J$10,CONCATENATE("Winner Match #",$A$10),IF($H$10&gt;$J$10,$E$10,$G$10))</f>
-        <v>Winner Match #9</v>
+        <v>Loser Match #2</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>7</v>
@@ -3609,7 +3599,7 @@
     </row>
     <row r="22" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -3665,7 +3655,7 @@
     </row>
     <row r="23" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -3721,7 +3711,7 @@
     </row>
     <row r="24" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="7">
@@ -3777,7 +3767,7 @@
     </row>
     <row r="25" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="6">
@@ -3833,7 +3823,7 @@
     </row>
     <row r="26" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="7">
@@ -3889,7 +3879,7 @@
     </row>
     <row r="27" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="6">
@@ -3945,7 +3935,7 @@
     </row>
     <row r="28" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -4001,7 +3991,7 @@
     </row>
     <row r="29" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
@@ -4057,7 +4047,7 @@
     </row>
     <row r="30" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" s="106" t="s">
@@ -4113,7 +4103,7 @@
     </row>
     <row r="31" spans="1:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -4186,8 +4176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E65B55-65C4-4E99-BEFB-6647B9FBC277}">
   <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S30" sqref="S1:S30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4275,10 +4265,10 @@
         <v>End time</v>
       </c>
       <c r="R1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -4304,15 +4294,15 @@
       </c>
       <c r="F2" t="str">
         <f>Resultate!G2</f>
-        <v>Dürst / Dürst</v>
-      </c>
-      <c r="G2" t="str">
+        <v>bye / bye</v>
+      </c>
+      <c r="G2">
         <f>Resultate!H2</f>
-        <v/>
-      </c>
-      <c r="H2" t="str">
+        <v>2</v>
+      </c>
+      <c r="H2">
         <f>Resultate!J2</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I2" s="132">
         <f>Resultate!K2</f>
@@ -4367,10 +4357,10 @@
 IF(_xlpm.blanksAfter=1,"in_progress","upcoming_"&amp;(_xlpm.blanksAfter-1)&amp;"_court"&amp;_xlpm.court)
 )
 ))</f>
-        <v>in_progress</v>
+        <v>completed</v>
       </c>
       <c r="S2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -4462,7 +4452,7 @@
         <v>in_progress</v>
       </c>
       <c r="S3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -4554,7 +4544,7 @@
         <v>in_progress</v>
       </c>
       <c r="S4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -4567,8 +4557,7 @@
         <v>I</v>
       </c>
       <c r="C5">
-        <f>Resultate!C5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="132">
         <f>Resultate!D5</f>
@@ -4643,10 +4632,10 @@
 IF(_xlpm.blanksAfter=1,"in_progress","upcoming_"&amp;(_xlpm.blanksAfter-1)&amp;"_court"&amp;_xlpm.court)
 )
 ))</f>
-        <v/>
+        <v>in_progress</v>
       </c>
       <c r="S5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -4738,7 +4727,7 @@
         <v/>
       </c>
       <c r="S6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -4830,7 +4819,7 @@
         <v/>
       </c>
       <c r="S7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -4922,7 +4911,7 @@
         <v/>
       </c>
       <c r="S8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -5014,7 +5003,7 @@
         <v/>
       </c>
       <c r="S9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -5036,19 +5025,19 @@
       </c>
       <c r="E10" t="str">
         <f>Resultate!E10</f>
-        <v>Loser Match #1</v>
+        <v>bye / bye</v>
       </c>
       <c r="F10" t="str">
         <f>Resultate!G10</f>
         <v>Loser Match #2</v>
       </c>
-      <c r="G10" t="str">
+      <c r="G10">
         <f>Resultate!H10</f>
-        <v/>
-      </c>
-      <c r="H10" t="str">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <f>Resultate!J10</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I10" s="132">
         <f>Resultate!K10</f>
@@ -5106,7 +5095,7 @@
         <v/>
       </c>
       <c r="S10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -5198,7 +5187,7 @@
         <v/>
       </c>
       <c r="S11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -5290,7 +5279,7 @@
         <v/>
       </c>
       <c r="S12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -5382,7 +5371,7 @@
         <v/>
       </c>
       <c r="S13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -5404,7 +5393,7 @@
       </c>
       <c r="E14" t="str">
         <f>Resultate!E14</f>
-        <v>Winner Match #1</v>
+        <v>Baltermi / Hill Azpeitia</v>
       </c>
       <c r="F14" t="str">
         <f>Resultate!G14</f>
@@ -5474,7 +5463,7 @@
         <v/>
       </c>
       <c r="S14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -5566,7 +5555,7 @@
         <v/>
       </c>
       <c r="S15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -5658,7 +5647,7 @@
         <v/>
       </c>
       <c r="S16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -5750,7 +5739,7 @@
         <v/>
       </c>
       <c r="S17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -5842,7 +5831,7 @@
         <v/>
       </c>
       <c r="S18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -5934,7 +5923,7 @@
         <v/>
       </c>
       <c r="S19" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -6026,7 +6015,7 @@
         <v/>
       </c>
       <c r="S20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -6048,7 +6037,7 @@
       </c>
       <c r="E21" t="str">
         <f>Resultate!E21</f>
-        <v>Winner Match #9</v>
+        <v>Loser Match #2</v>
       </c>
       <c r="F21" t="str">
         <f>Resultate!G21</f>
@@ -6118,7 +6107,7 @@
         <v/>
       </c>
       <c r="S21" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -6210,7 +6199,7 @@
         <v/>
       </c>
       <c r="S22" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -6302,7 +6291,7 @@
         <v/>
       </c>
       <c r="S23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -6394,7 +6383,7 @@
         <v/>
       </c>
       <c r="S24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -6486,7 +6475,7 @@
         <v/>
       </c>
       <c r="S25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -6578,7 +6567,7 @@
         <v/>
       </c>
       <c r="S26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -6670,7 +6659,7 @@
         <v/>
       </c>
       <c r="S27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -6762,7 +6751,7 @@
         <v/>
       </c>
       <c r="S28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -6854,7 +6843,7 @@
         <v/>
       </c>
       <c r="S29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -6946,7 +6935,7 @@
         <v/>
       </c>
       <c r="S30" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -7010,7 +6999,7 @@
       </c>
       <c r="B3" s="108" t="str">
         <f>CONCATENATE(Resultate!$E$14," ")</f>
-        <v xml:space="preserve">Winner Match #1 </v>
+        <v xml:space="preserve">Baltermi / Hill Azpeitia </v>
       </c>
       <c r="C3"/>
       <c r="D3" s="14"/>
@@ -7026,7 +7015,7 @@
     <row r="4" spans="1:14" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="str">
         <f>CONCATENATE("(",Resultate!$H$2," : ",Resultate!$J$2,")")</f>
-        <v>( : )</v>
+        <v>(2 : 0)</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4"/>
@@ -7043,7 +7032,7 @@
     <row r="5" spans="1:14" ht="9.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="110" t="str">
         <f>CONCATENATE(Resultate!$G$2," ")</f>
-        <v xml:space="preserve">Dürst / Dürst </v>
+        <v xml:space="preserve">bye / bye </v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5"/>
@@ -7847,7 +7836,7 @@
       <c r="H42" s="24"/>
       <c r="I42" s="116" t="str">
         <f>CONCATENATE(Resultate!$E$21," ")</f>
-        <v xml:space="preserve">Winner Match #9 </v>
+        <v xml:space="preserve">Loser Match #2 </v>
       </c>
       <c r="J42" s="21" t="str">
         <f>CONCATENATE("",Resultate!$A$10,"")</f>
@@ -7874,7 +7863,7 @@
       <c r="I43" s="118"/>
       <c r="J43" s="23" t="str">
         <f>CONCATENATE("(",Resultate!$J$10," : ",Resultate!$H$10,")")</f>
-        <v>( : )</v>
+        <v>(2 : 0)</v>
       </c>
       <c r="K43" s="9"/>
     </row>
@@ -7896,7 +7885,7 @@
       </c>
       <c r="J44" s="119" t="str">
         <f>CONCATENATE(Resultate!$E$10," ")</f>
-        <v xml:space="preserve">Loser Match #1 </v>
+        <v xml:space="preserve">bye / bye </v>
       </c>
       <c r="K44" s="9"/>
     </row>
@@ -8219,15 +8208,15 @@
       </c>
       <c r="B14" s="2" t="str">
         <f>IF(Resultate!$H$10=Resultate!$J$10,"13. Rang",IF(Resultate!$H$10&lt;Resultate!$J$10,Resultate!$E$10,Resultate!$G$10))</f>
-        <v>13. Rang</v>
+        <v>bye / bye</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>IF(B14="13. Rang","mal schauen",VLOOKUP(B14,Anmeldung!$L$2:$M$17,2,FALSE))</f>
-        <v>mal schauen</v>
-      </c>
-      <c r="D14" s="44" t="str">
+        <v>bye bye / bye bye</v>
+      </c>
+      <c r="D14" s="44">
         <f>IF(B14="13. Rang","zu Hause",VLOOKUP(B14,Anmeldung!$I$2:$J$17,2,FALSE))</f>
-        <v>zu Hause</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8300,26 +8289,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d704cbfe-ff76-4611-8b34-db3dc32c7f3e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a67d4247-ceba-4b8b-b2e1-e106cd044048">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100D9214984AE3BD84C9E574E78850AAA3B" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="6369a39dc7aedec7fd62eeb0a289445a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a67d4247-ceba-4b8b-b2e1-e106cd044048" xmlns:ns3="d704cbfe-ff76-4611-8b34-db3dc32c7f3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9d3638ed41143bbf6a5e0a931dae7110" ns2:_="" ns3:_="">
     <xsd:import namespace="a67d4247-ceba-4b8b-b2e1-e106cd044048"/>
@@ -8548,10 +8517,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d704cbfe-ff76-4611-8b34-db3dc32c7f3e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a67d4247-ceba-4b8b-b2e1-e106cd044048">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA0585E-29EC-48FB-AE84-B1F7932E2417}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E384A2-CB97-4FA1-A706-347B67FB7B7A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a67d4247-ceba-4b8b-b2e1-e106cd044048"/>
+    <ds:schemaRef ds:uri="d704cbfe-ff76-4611-8b34-db3dc32c7f3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8568,20 +8568,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43E384A2-CB97-4FA1-A706-347B67FB7B7A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BA0585E-29EC-48FB-AE84-B1F7932E2417}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a67d4247-ceba-4b8b-b2e1-e106cd044048"/>
-    <ds:schemaRef ds:uri="d704cbfe-ff76-4611-8b34-db3dc32c7f3e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>